<commit_message>
Improvised the cacheing of Question/Answer/ApplicationData
* Refactored for better caching.
* Updated the doc-slicing operations.
* Code cleanup
</commit_message>
<xml_diff>
--- a/resources/data_input.xlsx
+++ b/resources/data_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
     <t>Template</t>
   </si>
   <si>
-    <t>Ruchi Sharma</t>
+    <t>ThinkPad v1.5.22</t>
   </si>
 </sst>
 </file>
@@ -1017,18 +1017,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="108.7109375" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="108.7265625" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1551,12 +1551,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>28</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -1597,37 +1597,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>44</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>44</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>44</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>44</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>44</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>44</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>44</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>44</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>44</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>44</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>50</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>50</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>50</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>50</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>50</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>50</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>50</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>50</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>50</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>50</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>50</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>50</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>50</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>50</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>50</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>56</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>56</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>56</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>56</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>56</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>56</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>56</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>56</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>56</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>56</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>56</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>56</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>56</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>56</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>56</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>56</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>56</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>59</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>59</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>59</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>59</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>59</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>61</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>61</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>61</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>61</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>61</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>61</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>61</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>61</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>61</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>61</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>61</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>61</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>61</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>61</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>61</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>61</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>61</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>61</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>61</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>61</v>
       </c>
@@ -2835,27 +2835,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C177" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C178" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C179" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C180" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>63</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>63</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>63</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>63</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>63</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>63</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>63</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>63</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>63</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>70</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>70</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>70</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>70</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>70</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>70</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>70</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>70</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>70</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>70</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>70</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>70</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>70</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>70</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>70</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>70</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>70</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>70</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>70</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>70</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>70</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>75</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>75</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>75</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>75</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>75</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>75</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>75</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>75</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>75</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>75</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>75</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>75</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>75</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>75</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>75</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>75</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>75</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>75</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>77</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>77</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>77</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>77</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>77</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>77</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>77</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>77</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>77</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>77</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>77</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>77</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>77</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>77</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>77</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>77</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>77</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>77</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>77</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>77</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>80</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>80</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>80</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>80</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>80</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
         <v>96</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>80</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>80</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>80</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>80</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>80</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>80</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>80</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>80</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>80</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>80</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>80</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>80</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>80</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>80</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>80</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>81</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>81</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>81</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>81</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>81</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>81</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>81</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>81</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>81</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>81</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>81</v>
       </c>
@@ -3953,22 +3953,22 @@
         <v>82</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>81</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>81</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>81</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>81</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>81</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>81</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>81</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>81</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>81</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>81</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>86</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>86</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>86</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>86</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>86</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>86</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>86</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>86</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>86</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>86</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>86</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>86</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>86</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>86</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>86</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>86</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>86</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>86</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>86</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>86</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>86</v>
       </c>
@@ -4306,16 +4306,16 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.54296875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="11" t="s">
         <v>167</v>
@@ -4325,12 +4325,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>132</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>134</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>135</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>136</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>137</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>139</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>140</v>
       </c>
@@ -4424,67 +4424,67 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>153</v>
       </c>
@@ -4511,11 +4511,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delete operation & Answer Replacements
* Improvised the DELETE operation of H4-slices.
** Yet the Deleted paragraphs are displayed as blank lines.
* Refactored the creation of block-slices to a static method for
code-reuse.
* Introduced a DEFAULT field for questions in mapping excel.
* Updated the PROCESS module to handle:
** the Checkbox type of questions.
** linking of questions in case of 'Other' as answer.
** replacing of the global fields with all the answers (comma seperated)
* Code Cleanup and Standardization
</commit_message>
<xml_diff>
--- a/resources/data_input.xlsx
+++ b/resources/data_input.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="168">
   <si>
     <t>AP000293_Access CENTRAL</t>
   </si>
@@ -337,9 +337,6 @@
     <t>What Protocol Authentication mechanism, if any, does this application use?</t>
   </si>
   <si>
-    <t>NTLM,Kerberos</t>
-  </si>
-  <si>
     <t>If you select "Other" for the Protocol mechanism method, specify the protocol used.</t>
   </si>
   <si>
@@ -446,9 +443,6 @@
   </si>
   <si>
     <t>leapdb.fmr.com, leapdbdev.fmr.com, Greg Cash, DMN1</t>
-  </si>
-  <si>
-    <t>Other0</t>
   </si>
   <si>
     <t>Q1</t>
@@ -604,7 +598,7 @@
     <t>Template</t>
   </si>
   <si>
-    <t>ThinkPad v1.5.22</t>
+    <t>NTLM,Kerberos,Oauth</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,9 +1040,7 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>169</v>
-      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1058,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1080,7 +1072,7 @@
         <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1088,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1097,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -1108,10 +1100,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1141,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -1150,10 +1142,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1183,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
@@ -1194,10 +1186,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1216,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -1225,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>17</v>
@@ -1247,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
@@ -1258,10 +1250,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1280,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1307,7 +1299,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1315,10 +1307,10 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1326,7 +1318,7 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
@@ -1351,7 +1343,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1359,7 +1351,7 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1367,7 +1359,7 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1400,7 +1392,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1408,7 +1400,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
@@ -1430,10 +1422,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1441,7 +1433,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -1463,7 +1455,7 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -1474,7 +1466,7 @@
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -1523,10 +1515,10 @@
         <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1534,7 +1526,7 @@
         <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -1545,7 +1537,7 @@
         <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
         <v>31</v>
@@ -1575,7 +1567,7 @@
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1583,7 +1575,7 @@
         <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1591,7 +1583,7 @@
         <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
@@ -1654,7 +1646,7 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
         <v>41</v>
@@ -1665,7 +1657,7 @@
         <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
         <v>42</v>
@@ -1687,10 +1679,10 @@
         <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1698,7 +1690,7 @@
         <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -1720,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
@@ -1731,7 +1723,7 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
@@ -1753,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1780,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1788,10 +1780,10 @@
         <v>44</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1799,10 +1791,10 @@
         <v>44</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1824,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1832,7 +1824,7 @@
         <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1840,7 +1832,7 @@
         <v>44</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
         <v>46</v>
@@ -1873,7 +1865,7 @@
         <v>44</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
         <v>47</v>
@@ -1884,7 +1876,7 @@
         <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
         <v>48</v>
@@ -1906,7 +1898,7 @@
         <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1914,7 +1906,7 @@
         <v>44</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -1936,7 +1928,7 @@
         <v>44</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C91" t="s">
         <v>27</v>
@@ -1947,7 +1939,7 @@
         <v>44</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C92" t="s">
         <v>49</v>
@@ -1972,7 +1964,7 @@
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1999,7 +1991,7 @@
         <v>50</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2007,7 +1999,7 @@
         <v>50</v>
       </c>
       <c r="B98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C98" t="s">
         <v>53</v>
@@ -2018,7 +2010,7 @@
         <v>50</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
         <v>45</v>
@@ -2051,7 +2043,7 @@
         <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -2059,7 +2051,7 @@
         <v>50</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C103" t="s">
         <v>54</v>
@@ -2092,7 +2084,7 @@
         <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -2100,7 +2092,7 @@
         <v>50</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C107" t="s">
         <v>22</v>
@@ -2122,7 +2114,7 @@
         <v>50</v>
       </c>
       <c r="B109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -2130,7 +2122,7 @@
         <v>50</v>
       </c>
       <c r="B110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C110" t="s">
         <v>7</v>
@@ -2152,7 +2144,7 @@
         <v>50</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
         <v>12</v>
@@ -2163,7 +2155,7 @@
         <v>50</v>
       </c>
       <c r="B113" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C113" t="s">
         <v>53</v>
@@ -2212,7 +2204,7 @@
         <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -2220,7 +2212,7 @@
         <v>56</v>
       </c>
       <c r="B119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C119" t="s">
         <v>53</v>
@@ -2231,7 +2223,7 @@
         <v>56</v>
       </c>
       <c r="B120" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C120" t="s">
         <v>12</v>
@@ -2264,7 +2256,7 @@
         <v>56</v>
       </c>
       <c r="B123" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -2272,7 +2264,7 @@
         <v>56</v>
       </c>
       <c r="B124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C124" t="s">
         <v>22</v>
@@ -2305,7 +2297,7 @@
         <v>56</v>
       </c>
       <c r="B127" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -2313,7 +2305,7 @@
         <v>56</v>
       </c>
       <c r="B128" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C128" t="s">
         <v>22</v>
@@ -2335,7 +2327,7 @@
         <v>56</v>
       </c>
       <c r="B130" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -2343,7 +2335,7 @@
         <v>56</v>
       </c>
       <c r="B131" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C131" t="s">
         <v>7</v>
@@ -2365,7 +2357,7 @@
         <v>56</v>
       </c>
       <c r="B133" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C133" t="s">
         <v>12</v>
@@ -2376,7 +2368,7 @@
         <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C134" t="s">
         <v>7</v>
@@ -2425,7 +2417,7 @@
         <v>59</v>
       </c>
       <c r="B139" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -2433,7 +2425,7 @@
         <v>59</v>
       </c>
       <c r="B140" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C140" t="s">
         <v>53</v>
@@ -2444,7 +2436,7 @@
         <v>59</v>
       </c>
       <c r="B141" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C141" t="s">
         <v>53</v>
@@ -2477,10 +2469,10 @@
         <v>59</v>
       </c>
       <c r="B144" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C144" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -2488,7 +2480,7 @@
         <v>59</v>
       </c>
       <c r="B145" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C145" t="s">
         <v>22</v>
@@ -2521,10 +2513,10 @@
         <v>59</v>
       </c>
       <c r="B148" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C148" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -2532,7 +2524,7 @@
         <v>59</v>
       </c>
       <c r="B149" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C149" t="s">
         <v>22</v>
@@ -2554,7 +2546,7 @@
         <v>59</v>
       </c>
       <c r="B151" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C151" t="s">
         <v>60</v>
@@ -2565,7 +2557,7 @@
         <v>59</v>
       </c>
       <c r="B152" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
@@ -2587,7 +2579,7 @@
         <v>59</v>
       </c>
       <c r="B154" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C154" t="s">
         <v>12</v>
@@ -2598,10 +2590,10 @@
         <v>59</v>
       </c>
       <c r="B155" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C155" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -2645,7 +2637,7 @@
         <v>93</v>
       </c>
       <c r="C159" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -2653,7 +2645,7 @@
         <v>61</v>
       </c>
       <c r="B160" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C160" t="s">
         <v>62</v>
@@ -2664,7 +2656,7 @@
         <v>61</v>
       </c>
       <c r="B161" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C161" t="s">
         <v>62</v>
@@ -2675,7 +2667,7 @@
         <v>61</v>
       </c>
       <c r="B162" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C162" t="s">
         <v>62</v>
@@ -2708,7 +2700,7 @@
         <v>61</v>
       </c>
       <c r="B165" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C165" t="s">
         <v>62</v>
@@ -2719,7 +2711,7 @@
         <v>61</v>
       </c>
       <c r="B166" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C166" t="s">
         <v>62</v>
@@ -2752,7 +2744,7 @@
         <v>61</v>
       </c>
       <c r="B169" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C169" t="s">
         <v>62</v>
@@ -2763,7 +2755,7 @@
         <v>61</v>
       </c>
       <c r="B170" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C170" t="s">
         <v>62</v>
@@ -2785,7 +2777,7 @@
         <v>61</v>
       </c>
       <c r="B172" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C172" t="s">
         <v>62</v>
@@ -2796,7 +2788,7 @@
         <v>61</v>
       </c>
       <c r="B173" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C173" t="s">
         <v>7</v>
@@ -2818,7 +2810,7 @@
         <v>61</v>
       </c>
       <c r="B175" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C175" t="s">
         <v>12</v>
@@ -2829,7 +2821,7 @@
         <v>61</v>
       </c>
       <c r="B176" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C176" t="s">
         <v>62</v>
@@ -2882,7 +2874,7 @@
         <v>63</v>
       </c>
       <c r="B183" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
@@ -2890,7 +2882,7 @@
         <v>63</v>
       </c>
       <c r="B184" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C184" t="s">
         <v>69</v>
@@ -2912,7 +2904,7 @@
         <v>63</v>
       </c>
       <c r="B186" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
@@ -2920,7 +2912,7 @@
         <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C187" t="s">
         <v>17</v>
@@ -2942,7 +2934,7 @@
         <v>63</v>
       </c>
       <c r="B189" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C189" t="s">
         <v>20</v>
@@ -2953,10 +2945,10 @@
         <v>63</v>
       </c>
       <c r="B190" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C190" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
@@ -3002,7 +2994,7 @@
         <v>70</v>
       </c>
       <c r="B195" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -3010,7 +3002,7 @@
         <v>70</v>
       </c>
       <c r="B196" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C196" t="s">
         <v>53</v>
@@ -3021,7 +3013,7 @@
         <v>70</v>
       </c>
       <c r="B197" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C197" t="s">
         <v>22</v>
@@ -3054,7 +3046,7 @@
         <v>70</v>
       </c>
       <c r="B200" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C200" t="s">
         <v>22</v>
@@ -3065,7 +3057,7 @@
         <v>70</v>
       </c>
       <c r="B201" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C201" t="s">
         <v>22</v>
@@ -3098,7 +3090,7 @@
         <v>70</v>
       </c>
       <c r="B204" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -3106,7 +3098,7 @@
         <v>70</v>
       </c>
       <c r="B205" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C205" t="s">
         <v>22</v>
@@ -3128,7 +3120,7 @@
         <v>70</v>
       </c>
       <c r="B207" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -3136,7 +3128,7 @@
         <v>70</v>
       </c>
       <c r="B208" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C208" t="s">
         <v>7</v>
@@ -3158,7 +3150,7 @@
         <v>70</v>
       </c>
       <c r="B210" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C210" t="s">
         <v>12</v>
@@ -3169,7 +3161,7 @@
         <v>70</v>
       </c>
       <c r="B211" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C211" t="s">
         <v>53</v>
@@ -3221,7 +3213,7 @@
         <v>75</v>
       </c>
       <c r="B216" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -3229,7 +3221,7 @@
         <v>75</v>
       </c>
       <c r="B217" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C217" t="s">
         <v>53</v>
@@ -3240,7 +3232,7 @@
         <v>75</v>
       </c>
       <c r="B218" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C218" t="s">
         <v>53</v>
@@ -3273,7 +3265,7 @@
         <v>75</v>
       </c>
       <c r="B221" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C221" t="s">
         <v>76</v>
@@ -3284,7 +3276,7 @@
         <v>75</v>
       </c>
       <c r="B222" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C222" t="s">
         <v>12</v>
@@ -3317,7 +3309,7 @@
         <v>75</v>
       </c>
       <c r="B225" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C225" t="s">
         <v>12</v>
@@ -3328,7 +3320,7 @@
         <v>75</v>
       </c>
       <c r="B226" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C226" t="s">
         <v>12</v>
@@ -3350,7 +3342,7 @@
         <v>75</v>
       </c>
       <c r="B228" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -3358,7 +3350,7 @@
         <v>75</v>
       </c>
       <c r="B229" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C229" t="s">
         <v>7</v>
@@ -3380,7 +3372,7 @@
         <v>75</v>
       </c>
       <c r="B231" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C231" t="s">
         <v>12</v>
@@ -3391,7 +3383,7 @@
         <v>75</v>
       </c>
       <c r="B232" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C232" t="s">
         <v>12</v>
@@ -3405,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="C233" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -3443,7 +3435,7 @@
         <v>77</v>
       </c>
       <c r="B237" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -3451,7 +3443,7 @@
         <v>77</v>
       </c>
       <c r="B238" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C238" t="s">
         <v>53</v>
@@ -3462,7 +3454,7 @@
         <v>77</v>
       </c>
       <c r="B239" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C239" t="s">
         <v>12</v>
@@ -3495,7 +3487,7 @@
         <v>77</v>
       </c>
       <c r="B242" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
@@ -3503,7 +3495,7 @@
         <v>77</v>
       </c>
       <c r="B243" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C243" t="s">
         <v>22</v>
@@ -3536,7 +3528,7 @@
         <v>77</v>
       </c>
       <c r="B246" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C246" t="s">
         <v>78</v>
@@ -3547,7 +3539,7 @@
         <v>77</v>
       </c>
       <c r="B247" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C247" t="s">
         <v>22</v>
@@ -3569,7 +3561,7 @@
         <v>77</v>
       </c>
       <c r="B249" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C249" t="s">
         <v>73</v>
@@ -3580,7 +3572,7 @@
         <v>77</v>
       </c>
       <c r="B250" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C250" t="s">
         <v>80</v>
@@ -3602,7 +3594,7 @@
         <v>77</v>
       </c>
       <c r="B252" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C252" t="s">
         <v>12</v>
@@ -3613,7 +3605,7 @@
         <v>77</v>
       </c>
       <c r="B253" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C253" t="s">
         <v>79</v>
@@ -3627,7 +3619,7 @@
         <v>1</v>
       </c>
       <c r="C254" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -3668,7 +3660,7 @@
         <v>80</v>
       </c>
       <c r="B258" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C258" t="s">
         <v>74</v>
@@ -3676,7 +3668,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C260" t="s">
         <v>74</v>
@@ -3687,7 +3679,7 @@
         <v>80</v>
       </c>
       <c r="B262" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C262" t="s">
         <v>12</v>
@@ -3720,7 +3712,7 @@
         <v>80</v>
       </c>
       <c r="B265" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C265" t="s">
         <v>73</v>
@@ -3731,7 +3723,7 @@
         <v>80</v>
       </c>
       <c r="B266" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C266" t="s">
         <v>74</v>
@@ -3764,10 +3756,10 @@
         <v>80</v>
       </c>
       <c r="B270" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C270" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
@@ -3775,7 +3767,7 @@
         <v>80</v>
       </c>
       <c r="B271" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C271" t="s">
         <v>12</v>
@@ -3797,7 +3789,7 @@
         <v>80</v>
       </c>
       <c r="B273" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
@@ -3805,7 +3797,7 @@
         <v>80</v>
       </c>
       <c r="B274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C274" t="s">
         <v>17</v>
@@ -3827,7 +3819,7 @@
         <v>80</v>
       </c>
       <c r="B276" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C276" t="s">
         <v>12</v>
@@ -3838,7 +3830,7 @@
         <v>80</v>
       </c>
       <c r="B277" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C277" t="s">
         <v>12</v>
@@ -3887,7 +3879,7 @@
         <v>81</v>
       </c>
       <c r="B282" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
@@ -3895,7 +3887,7 @@
         <v>81</v>
       </c>
       <c r="B283" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C283" t="s">
         <v>53</v>
@@ -3906,10 +3898,10 @@
         <v>81</v>
       </c>
       <c r="B284" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C284" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
@@ -3939,7 +3931,7 @@
         <v>81</v>
       </c>
       <c r="B287" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
@@ -3947,7 +3939,7 @@
         <v>81</v>
       </c>
       <c r="B288" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C288" t="s">
         <v>82</v>
@@ -3995,7 +3987,7 @@
         <v>81</v>
       </c>
       <c r="B294" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
@@ -4003,7 +3995,7 @@
         <v>81</v>
       </c>
       <c r="B295" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C295" t="s">
         <v>22</v>
@@ -4025,7 +4017,7 @@
         <v>81</v>
       </c>
       <c r="B297" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.35">
@@ -4033,7 +4025,7 @@
         <v>81</v>
       </c>
       <c r="B298" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C298" t="s">
         <v>7</v>
@@ -4055,7 +4047,7 @@
         <v>81</v>
       </c>
       <c r="B300" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C300" t="s">
         <v>12</v>
@@ -4066,7 +4058,7 @@
         <v>81</v>
       </c>
       <c r="B301" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C301" t="s">
         <v>7</v>
@@ -4118,7 +4110,7 @@
         <v>86</v>
       </c>
       <c r="B306" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
@@ -4126,7 +4118,7 @@
         <v>86</v>
       </c>
       <c r="B307" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C307" t="s">
         <v>53</v>
@@ -4137,7 +4129,7 @@
         <v>86</v>
       </c>
       <c r="B308" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C308" t="s">
         <v>12</v>
@@ -4170,7 +4162,7 @@
         <v>86</v>
       </c>
       <c r="B311" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
@@ -4178,7 +4170,7 @@
         <v>86</v>
       </c>
       <c r="B312" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C312" t="s">
         <v>22</v>
@@ -4211,7 +4203,7 @@
         <v>86</v>
       </c>
       <c r="B315" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C315" t="s">
         <v>87</v>
@@ -4222,7 +4214,7 @@
         <v>86</v>
       </c>
       <c r="B316" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C316" t="s">
         <v>7</v>
@@ -4244,7 +4236,7 @@
         <v>86</v>
       </c>
       <c r="B318" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.35">
@@ -4252,7 +4244,7 @@
         <v>86</v>
       </c>
       <c r="B319" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C319" t="s">
         <v>7</v>
@@ -4274,7 +4266,7 @@
         <v>86</v>
       </c>
       <c r="B321" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C321" t="s">
         <v>12</v>
@@ -4285,7 +4277,7 @@
         <v>86</v>
       </c>
       <c r="B322" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C322" t="s">
         <v>17</v>
@@ -4318,32 +4310,32 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4">
         <v>4.16</v>
@@ -4351,21 +4343,21 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6">
         <v>4.12</v>
@@ -4373,120 +4365,120 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D8">
         <v>4.2</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D9">
         <v>4.7</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored multiple scenarios of CHECKBOX & RADIO questions
* Introduced the accomodation of content from answer of 'Other'
question, to the comma seperated values.
* Analyzed the updates needed to question-mapping:
** Updated the processing for RADIO type of questions.
* Code Cleanup.
</commit_message>
<xml_diff>
--- a/resources/data_input.xlsx
+++ b/resources/data_input.xlsx
@@ -635,7 +635,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +645,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,7 +684,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -705,6 +710,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1023,236 +1029,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4300,20 +4306,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.54296875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.54296875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
     <col min="5" max="5" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4323,18 +4329,18 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>152</v>
       </c>
       <c r="D4">
@@ -4342,21 +4348,21 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>154</v>
       </c>
       <c r="D6">
@@ -4364,21 +4370,21 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>161</v>
       </c>
       <c r="D8">
@@ -4389,27 +4395,27 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>162</v>
       </c>
       <c r="D9">
         <v>4.7</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>163</v>
       </c>
       <c r="E10" t="s">
@@ -4417,67 +4423,67 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the large-text to default content
* Removed few radio components and made them static text.
* Fixed the AttributeError in setting doc-header contents by introducing EnsureDispatch
* Wrapped the code of document-decoration in try-expect.
* Code Cleanup
</commit_message>
<xml_diff>
--- a/resources/data_input.xlsx
+++ b/resources/data_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="167">
   <si>
     <t>AP000293_Access CENTRAL</t>
   </si>
@@ -377,9 +377,6 @@
   </si>
   <si>
     <t>Does the application utilize a dedicated/common Data repository such as Sharepoint, DocumentCentral, Confluence, etc?</t>
-  </si>
-  <si>
-    <t>SharePoint, Confluence, Bit Bucket, edms</t>
   </si>
   <si>
     <t>Authentication - Service  Accounts,Centrify</t>
@@ -598,7 +595,7 @@
     <t>Template</t>
   </si>
   <si>
-    <t>NTLM,Kerberos,Oauth</t>
+    <t>Distribution List and Shared Mailbox</t>
   </si>
 </sst>
 </file>
@@ -707,10 +704,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,29 +1014,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-    <col min="2" max="2" width="108.7265625" customWidth="1"/>
-    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="108.7109375" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1045,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,10 +1075,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1087,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1109,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1140,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1151,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1195,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1215,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1248,10 +1245,10 @@
         <v>106</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1259,10 +1256,10 @@
         <v>107</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1278,10 +1275,10 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1308,7 +1305,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1316,10 +1313,10 @@
         <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1349,10 +1346,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1360,7 +1357,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1382,7 +1379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1393,7 +1390,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1401,7 +1398,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1412,7 +1409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -1423,7 +1420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -1431,10 +1428,10 @@
         <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -1445,7 +1442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1456,7 +1453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1467,7 +1464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1486,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1497,7 +1494,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -1505,7 +1502,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1524,10 +1521,10 @@
         <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1549,12 +1546,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>28</v>
       </c>
@@ -1565,7 +1562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1573,10 +1570,10 @@
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -1584,7 +1581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -1595,37 +1592,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -1647,7 +1644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -1669,7 +1666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -1688,10 +1685,10 @@
         <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -1702,7 +1699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -1713,7 +1710,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -1735,7 +1732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>44</v>
       </c>
@@ -1743,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>44</v>
       </c>
@@ -1751,10 +1748,10 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>44</v>
       </c>
@@ -1762,7 +1759,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -1781,7 +1778,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>44</v>
       </c>
@@ -1789,10 +1786,10 @@
         <v>95</v>
       </c>
       <c r="C77" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>44</v>
       </c>
@@ -1800,10 +1797,10 @@
         <v>96</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>44</v>
       </c>
@@ -1814,7 +1811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>44</v>
       </c>
@@ -1822,10 +1819,10 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -1833,7 +1830,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -1844,7 +1841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -1877,7 +1874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>44</v>
       </c>
@@ -1888,7 +1885,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>44</v>
       </c>
@@ -1899,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -1918,7 +1915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -1929,7 +1926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -1940,7 +1937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -1951,7 +1948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>50</v>
       </c>
@@ -1962,7 +1959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>50</v>
       </c>
@@ -1970,10 +1967,10 @@
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>50</v>
       </c>
@@ -1981,7 +1978,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -1992,7 +1989,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>50</v>
       </c>
@@ -2000,7 +1997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -2011,7 +2008,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>50</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>50</v>
       </c>
@@ -2033,7 +2030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>50</v>
       </c>
@@ -2044,7 +2041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2052,7 +2049,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -2063,7 +2060,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>50</v>
       </c>
@@ -2074,7 +2071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>50</v>
       </c>
@@ -2085,7 +2082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -2093,7 +2090,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>50</v>
       </c>
@@ -2104,7 +2101,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>50</v>
       </c>
@@ -2115,7 +2112,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>50</v>
       </c>
@@ -2123,7 +2120,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>50</v>
       </c>
@@ -2134,7 +2131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>50</v>
       </c>
@@ -2145,7 +2142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>50</v>
       </c>
@@ -2156,7 +2153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>50</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>56</v>
       </c>
@@ -2175,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>56</v>
       </c>
@@ -2186,7 +2183,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>56</v>
       </c>
@@ -2194,7 +2191,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>56</v>
       </c>
@@ -2205,7 +2202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>56</v>
       </c>
@@ -2213,7 +2210,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>56</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -2235,7 +2232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>56</v>
       </c>
@@ -2246,7 +2243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -2257,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -2265,7 +2262,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>56</v>
       </c>
@@ -2287,7 +2284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>56</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2303,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>56</v>
       </c>
@@ -2317,7 +2314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>56</v>
       </c>
@@ -2328,7 +2325,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>56</v>
       </c>
@@ -2336,7 +2333,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>56</v>
       </c>
@@ -2347,7 +2344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>56</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>56</v>
       </c>
@@ -2369,7 +2366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>56</v>
       </c>
@@ -2380,7 +2377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -2388,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -2407,7 +2404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -2418,7 +2415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -2426,7 +2423,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -2437,7 +2434,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -2448,7 +2445,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>59</v>
       </c>
@@ -2459,7 +2456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>59</v>
       </c>
@@ -2470,7 +2467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>59</v>
       </c>
@@ -2478,10 +2475,10 @@
         <v>98</v>
       </c>
       <c r="C144" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>59</v>
       </c>
@@ -2492,7 +2489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>59</v>
       </c>
@@ -2503,7 +2500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -2514,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -2522,10 +2519,10 @@
         <v>101</v>
       </c>
       <c r="C148" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -2536,7 +2533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -2547,7 +2544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -2558,7 +2555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -2569,7 +2566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -2580,7 +2577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -2591,7 +2588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -2599,10 +2596,10 @@
         <v>107</v>
       </c>
       <c r="C155" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -2613,7 +2610,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>61</v>
       </c>
@@ -2624,7 +2621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>61</v>
       </c>
@@ -2635,7 +2632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>61</v>
       </c>
@@ -2643,10 +2640,10 @@
         <v>93</v>
       </c>
       <c r="C159" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>61</v>
       </c>
@@ -2657,7 +2654,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>61</v>
       </c>
@@ -2668,7 +2665,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>61</v>
       </c>
@@ -2679,7 +2676,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>61</v>
       </c>
@@ -2690,7 +2687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>61</v>
       </c>
@@ -2701,7 +2698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>61</v>
       </c>
@@ -2712,7 +2709,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>61</v>
       </c>
@@ -2723,7 +2720,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>61</v>
       </c>
@@ -2734,7 +2731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>61</v>
       </c>
@@ -2745,7 +2742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>61</v>
       </c>
@@ -2756,7 +2753,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>61</v>
       </c>
@@ -2767,7 +2764,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>61</v>
       </c>
@@ -2778,7 +2775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>61</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>61</v>
       </c>
@@ -2800,7 +2797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>61</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>61</v>
       </c>
@@ -2822,7 +2819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>61</v>
       </c>
@@ -2833,27 +2830,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C180" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>63</v>
       </c>
@@ -2864,7 +2861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>63</v>
       </c>
@@ -2875,7 +2872,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>63</v>
       </c>
@@ -2883,7 +2880,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>63</v>
       </c>
@@ -2894,7 +2891,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>63</v>
       </c>
@@ -2905,7 +2902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>63</v>
       </c>
@@ -2913,7 +2910,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>63</v>
       </c>
@@ -2924,7 +2921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -2935,7 +2932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>63</v>
       </c>
@@ -2946,7 +2943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>63</v>
       </c>
@@ -2954,10 +2951,10 @@
         <v>107</v>
       </c>
       <c r="C190" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>70</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>70</v>
       </c>
@@ -2976,7 +2973,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>70</v>
       </c>
@@ -2984,7 +2981,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>70</v>
       </c>
@@ -2995,7 +2992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>70</v>
       </c>
@@ -3003,7 +3000,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>70</v>
       </c>
@@ -3014,7 +3011,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>70</v>
       </c>
@@ -3025,7 +3022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>70</v>
       </c>
@@ -3036,7 +3033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>70</v>
       </c>
@@ -3047,7 +3044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>70</v>
       </c>
@@ -3058,7 +3055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>70</v>
       </c>
@@ -3069,7 +3066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>70</v>
       </c>
@@ -3080,7 +3077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>70</v>
       </c>
@@ -3091,7 +3088,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>70</v>
       </c>
@@ -3099,7 +3096,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>70</v>
       </c>
@@ -3110,7 +3107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>70</v>
       </c>
@@ -3121,7 +3118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>70</v>
       </c>
@@ -3129,7 +3126,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>70</v>
       </c>
@@ -3140,7 +3137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>70</v>
       </c>
@@ -3151,7 +3148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>70</v>
       </c>
@@ -3162,7 +3159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>70</v>
       </c>
@@ -3173,7 +3170,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>75</v>
       </c>
@@ -3184,7 +3181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>75</v>
       </c>
@@ -3195,7 +3192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>75</v>
       </c>
@@ -3203,7 +3200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>75</v>
       </c>
@@ -3214,7 +3211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>75</v>
       </c>
@@ -3222,7 +3219,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>75</v>
       </c>
@@ -3233,7 +3230,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>75</v>
       </c>
@@ -3244,7 +3241,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>75</v>
       </c>
@@ -3255,7 +3252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>75</v>
       </c>
@@ -3266,7 +3263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>75</v>
       </c>
@@ -3277,7 +3274,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -3288,7 +3285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>75</v>
       </c>
@@ -3299,7 +3296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>75</v>
       </c>
@@ -3310,7 +3307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>75</v>
       </c>
@@ -3321,7 +3318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -3332,7 +3329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>75</v>
       </c>
@@ -3343,7 +3340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>75</v>
       </c>
@@ -3351,7 +3348,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>75</v>
       </c>
@@ -3362,7 +3359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>75</v>
       </c>
@@ -3373,7 +3370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>75</v>
       </c>
@@ -3384,7 +3381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -3395,7 +3392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>77</v>
       </c>
@@ -3403,10 +3400,10 @@
         <v>1</v>
       </c>
       <c r="C233" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>77</v>
       </c>
@@ -3417,7 +3414,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>77</v>
       </c>
@@ -3425,7 +3422,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>77</v>
       </c>
@@ -3436,7 +3433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>77</v>
       </c>
@@ -3444,7 +3441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>77</v>
       </c>
@@ -3455,7 +3452,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>77</v>
       </c>
@@ -3466,7 +3463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>77</v>
       </c>
@@ -3477,7 +3474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>77</v>
       </c>
@@ -3488,7 +3485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>77</v>
       </c>
@@ -3496,7 +3493,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>77</v>
       </c>
@@ -3507,7 +3504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>77</v>
       </c>
@@ -3518,7 +3515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>77</v>
       </c>
@@ -3529,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -3540,7 +3537,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>77</v>
       </c>
@@ -3551,7 +3548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>77</v>
       </c>
@@ -3562,7 +3559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>77</v>
       </c>
@@ -3573,7 +3570,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>77</v>
       </c>
@@ -3584,7 +3581,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>77</v>
       </c>
@@ -3595,7 +3592,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>77</v>
       </c>
@@ -3606,7 +3603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>77</v>
       </c>
@@ -3617,7 +3614,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>80</v>
       </c>
@@ -3625,10 +3622,10 @@
         <v>1</v>
       </c>
       <c r="C254" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>80</v>
       </c>
@@ -3639,7 +3636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>80</v>
       </c>
@@ -3650,7 +3647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>80</v>
       </c>
@@ -3661,7 +3658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>80</v>
       </c>
@@ -3672,7 +3669,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
         <v>95</v>
       </c>
@@ -3680,7 +3677,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>80</v>
       </c>
@@ -3691,7 +3688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>80</v>
       </c>
@@ -3702,7 +3699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>80</v>
       </c>
@@ -3713,7 +3710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>80</v>
       </c>
@@ -3724,7 +3721,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>80</v>
       </c>
@@ -3735,7 +3732,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>80</v>
       </c>
@@ -3746,7 +3743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>80</v>
       </c>
@@ -3757,7 +3754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>80</v>
       </c>
@@ -3765,10 +3762,10 @@
         <v>101</v>
       </c>
       <c r="C270" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>80</v>
       </c>
@@ -3779,7 +3776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>80</v>
       </c>
@@ -3790,7 +3787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>80</v>
       </c>
@@ -3798,7 +3795,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>80</v>
       </c>
@@ -3809,7 +3806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>80</v>
       </c>
@@ -3820,7 +3817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>80</v>
       </c>
@@ -3831,7 +3828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>80</v>
       </c>
@@ -3842,7 +3839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>81</v>
       </c>
@@ -3850,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>81</v>
       </c>
@@ -3861,7 +3858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>81</v>
       </c>
@@ -3869,7 +3866,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>81</v>
       </c>
@@ -3880,7 +3877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>81</v>
       </c>
@@ -3888,7 +3885,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>81</v>
       </c>
@@ -3899,7 +3896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>81</v>
       </c>
@@ -3907,10 +3904,10 @@
         <v>96</v>
       </c>
       <c r="C284" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>81</v>
       </c>
@@ -3921,7 +3918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>81</v>
       </c>
@@ -3932,7 +3929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>81</v>
       </c>
@@ -3940,7 +3937,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>81</v>
       </c>
@@ -3951,22 +3948,22 @@
         <v>82</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>81</v>
       </c>
@@ -3977,7 +3974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>81</v>
       </c>
@@ -3988,7 +3985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>81</v>
       </c>
@@ -3996,7 +3993,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>81</v>
       </c>
@@ -4007,7 +4004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>81</v>
       </c>
@@ -4018,7 +4015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>81</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>81</v>
       </c>
@@ -4037,7 +4034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>81</v>
       </c>
@@ -4048,7 +4045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>81</v>
       </c>
@@ -4059,7 +4056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>81</v>
       </c>
@@ -4070,7 +4067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>86</v>
       </c>
@@ -4081,7 +4078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>86</v>
       </c>
@@ -4092,7 +4089,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>86</v>
       </c>
@@ -4100,7 +4097,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>86</v>
       </c>
@@ -4111,7 +4108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>86</v>
       </c>
@@ -4119,7 +4116,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>86</v>
       </c>
@@ -4130,7 +4127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>86</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>86</v>
       </c>
@@ -4152,7 +4149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>86</v>
       </c>
@@ -4163,7 +4160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>86</v>
       </c>
@@ -4171,7 +4168,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>86</v>
       </c>
@@ -4182,7 +4179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>86</v>
       </c>
@@ -4193,7 +4190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>86</v>
       </c>
@@ -4204,7 +4201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>86</v>
       </c>
@@ -4215,7 +4212,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>86</v>
       </c>
@@ -4226,7 +4223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>86</v>
       </c>
@@ -4237,7 +4234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>86</v>
       </c>
@@ -4245,7 +4242,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>86</v>
       </c>
@@ -4256,7 +4253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>86</v>
       </c>
@@ -4267,7 +4264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>86</v>
       </c>
@@ -4278,7 +4275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>86</v>
       </c>
@@ -4304,187 +4301,187 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.54296875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="35.54296875" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="B4" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4">
         <v>4.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="B6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="D6">
         <v>4.12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>156</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8">
         <v>4.2</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9">
         <v>4.7</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -4509,11 +4506,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>